<commit_message>
dowload nao indo p pasta correta mas baixando certo em guia rapida
</commit_message>
<xml_diff>
--- a/EMPRESAS FGTS.xlsx
+++ b/EMPRESAS FGTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Hdlogika\k\Backup_19_08_2021\Unidade_D\K\LEATICIA\Luiz Fernando\Automacao_rfb\d-bitos_rfb_pr-mor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423B8A33-DD59-4B99-B4F4-2AE85428AA58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D898D4-0D1D-4BD9-8143-A6C732AA951A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="231">
   <si>
     <t>Código</t>
   </si>
@@ -711,6 +711,9 @@
   <si>
     <t>05.923.186/0001-74</t>
   </si>
+  <si>
+    <t>11.192.559/0001-87</t>
+  </si>
 </sst>
 </file>
 
@@ -719,7 +722,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00&quot;.&quot;000&quot;.&quot;000&quot;/&quot;0000&quot;-&quot;00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -735,6 +738,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -764,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -783,6 +793,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1035,7 +1046,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1119,8 +1130,8 @@
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>229</v>
+      <c r="C3" s="8" t="s">
+        <v>230</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1187,8 +1198,8 @@
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>229</v>
+      <c r="C5" s="8" t="s">
+        <v>230</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>

</xml_diff>

<commit_message>
digiliza achando a msg
</commit_message>
<xml_diff>
--- a/EMPRESAS FGTS.xlsx
+++ b/EMPRESAS FGTS.xlsx
@@ -808,10 +808,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">

</xml_diff>